<commit_message>
Updated mistake in README
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greenr/Documents/Teaching/Shells/CS_4170_5170_Parallel_Programming/Code/openMp/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C0AC02-9CDC-244C-BE64-320BF7D1B1A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01258930-8DA8-B449-81C6-51B4F53B0DCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{A5D04A24-9360-5747-ADEA-DF9E7E3AC58D}"/>
   </bookViews>
@@ -1224,6 +1224,8 @@
         <c:axId val="1636569855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3017,15 +3019,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>415193</xdr:colOff>
+      <xdr:colOff>356578</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>84016</xdr:rowOff>
+      <xdr:rowOff>74247</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>4885</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>776655</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>160216</xdr:rowOff>
+      <xdr:rowOff>150447</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3429,7 +3431,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>